<commit_message>
update group homework's template files
</commit_message>
<xml_diff>
--- a/bai-tap/bai-tap-nhom/test-case-thegioididong-backup.xlsx
+++ b/bai-tap/bai-tap-nhom/test-case-thegioididong-backup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\Hoc tap\Kiểm thử phần mềm\kiem-thu-phan-mem\bai-tap\bai-tap-nhom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D567C343-F663-4B2C-A268-28662C054DEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7F000A9-0974-4EBE-86A7-7F3F61E07B78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="79">
   <si>
     <t>1.    Phạm vi test</t>
   </si>
@@ -687,7 +687,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -807,6 +807,24 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -816,12 +834,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -834,18 +846,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -865,13 +865,2125 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="19" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="54">
+  <dxfs count="336">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1566,7 +3678,7 @@
   <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.09765625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1584,12 +3696,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="50" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="52"/>
+      <c r="A1" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="43"/>
       <c r="E1" s="8"/>
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
@@ -1617,11 +3729,11 @@
       <c r="G2" s="44" t="s">
         <v>62</v>
       </c>
-      <c r="H2" s="46" t="s">
+      <c r="H2" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="47"/>
-      <c r="J2" s="48" t="s">
+      <c r="I2" s="51"/>
+      <c r="J2" s="52" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1639,7 +3751,7 @@
       <c r="I3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="49"/>
+      <c r="J3" s="53"/>
     </row>
     <row r="4" spans="1:10" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9"/>
@@ -2133,11 +4245,11 @@
       <c r="J21" s="5"/>
     </row>
     <row r="22" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="50" t="s">
+      <c r="A22" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="51"/>
-      <c r="C22" s="53"/>
+      <c r="B22" s="42"/>
+      <c r="C22" s="46"/>
       <c r="D22" s="11"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
@@ -2170,7 +4282,7 @@
         <v>10</v>
       </c>
       <c r="D24" s="26">
-        <f>SUM(E4:E18)</f>
+        <f>COUNTIF('Test Case'!J:J,"Passed")</f>
         <v>0</v>
       </c>
       <c r="E24" s="12"/>
@@ -2187,7 +4299,7 @@
         <v>11</v>
       </c>
       <c r="D25" s="27">
-        <f>SUM(F4:F18)</f>
+        <f>COUNTIF('Test Case'!J:J,"Failed")</f>
         <v>0</v>
       </c>
       <c r="E25" s="12"/>
@@ -2204,10 +4316,10 @@
         <v>63</v>
       </c>
       <c r="D26" s="39">
-        <f>SUM(G4:G18)</f>
-        <v>0</v>
-      </c>
-      <c r="E26" s="5"/>
+        <f>COUNTIF('Test Case'!J:J,"Blocked")</f>
+        <v>0</v>
+      </c>
+      <c r="E26" s="12"/>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
@@ -2227,11 +4339,11 @@
       <c r="J27" s="5"/>
     </row>
     <row r="28" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="41" t="s">
+      <c r="A28" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="B28" s="42"/>
-      <c r="C28" s="43"/>
+      <c r="B28" s="48"/>
+      <c r="C28" s="49"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
@@ -2254,17 +4366,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="A22:C22"/>
     <mergeCell ref="A28:C28"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="J2:J3"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="F2:F3"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="A22:C22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
@@ -2278,9 +4390,9 @@
   </sheetPr>
   <dimension ref="A1:U88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L4" sqref="L4"/>
+      <selection pane="bottomLeft" activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.09765625" defaultRowHeight="32.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2313,6 +4425,15 @@
       <c r="I1" s="54"/>
       <c r="J1" s="54"/>
       <c r="K1" s="54"/>
+      <c r="M1" s="62" t="s">
+        <v>60</v>
+      </c>
+      <c r="N1" s="63" t="s">
+        <v>61</v>
+      </c>
+      <c r="O1" s="64" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="2" spans="1:21" s="32" customFormat="1" ht="34.799999999999997" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
@@ -2347,6 +4468,18 @@
       </c>
       <c r="K2" s="29" t="s">
         <v>23</v>
+      </c>
+      <c r="M2" s="61">
+        <f>COUNTIF(J:J,"Passed")</f>
+        <v>0</v>
+      </c>
+      <c r="N2" s="61">
+        <f>COUNTIF('Test Case'!J:J,"Failed")</f>
+        <v>0</v>
+      </c>
+      <c r="O2" s="61">
+        <f>COUNTIF('Test Case'!J:J,"Blocked")</f>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:21" s="33" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2999,244 +5132,391 @@
     <mergeCell ref="A19:K19"/>
   </mergeCells>
   <conditionalFormatting sqref="K4 K6 K8 K10 K12 K14 K16 K18 K1">
-    <cfRule type="containsText" dxfId="53" priority="207" operator="containsText" text="Blocked">
+    <cfRule type="containsText" dxfId="113" priority="267" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",K1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4 K6 K8 K10 K12 K14 K16 K18">
-    <cfRule type="containsText" dxfId="52" priority="205" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="112" priority="265" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",K4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="51" priority="206" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="111" priority="266" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",K4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K20">
-    <cfRule type="containsText" dxfId="50" priority="201" operator="containsText" text="Blocked">
+    <cfRule type="containsText" dxfId="110" priority="261" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",K20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K20">
-    <cfRule type="containsText" dxfId="49" priority="199" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="109" priority="259" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",K20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="48" priority="200" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="108" priority="260" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",K20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K22 K24 K26 K28">
-    <cfRule type="containsText" dxfId="47" priority="195" operator="containsText" text="Blocked">
+    <cfRule type="containsText" dxfId="107" priority="255" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",K22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K22 K24 K26 K28">
-    <cfRule type="containsText" dxfId="46" priority="193" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="106" priority="253" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",K22)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="194" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="105" priority="254" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",K22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K30">
-    <cfRule type="containsText" dxfId="44" priority="189" operator="containsText" text="Blocked">
+    <cfRule type="containsText" dxfId="104" priority="249" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",K30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K30">
-    <cfRule type="containsText" dxfId="43" priority="187" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="103" priority="247" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",K30)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="188" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="102" priority="248" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",K30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32">
-    <cfRule type="containsText" dxfId="41" priority="183" operator="containsText" text="Blocked">
+    <cfRule type="containsText" dxfId="101" priority="243" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",K32)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32">
-    <cfRule type="containsText" dxfId="40" priority="181" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="100" priority="241" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",K32)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="182" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="99" priority="242" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",K32)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K88">
-    <cfRule type="containsText" dxfId="38" priority="129" operator="containsText" text="Blocked">
+    <cfRule type="containsText" dxfId="98" priority="189" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",K88)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K88">
-    <cfRule type="containsText" dxfId="37" priority="127" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="97" priority="187" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",K88)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="128" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="96" priority="188" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",K88)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1 J3 J5 J7 J9 J11 J13 J15 J17 J19">
-    <cfRule type="containsText" dxfId="35" priority="126" operator="containsText" text="Blocked">
+    <cfRule type="containsText" dxfId="95" priority="186" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",J1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3 J5 J7 J9 J11 J13 J15 J17 J19">
-    <cfRule type="containsText" dxfId="34" priority="124" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="94" priority="184" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",J3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="125" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="93" priority="185" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",J3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J31">
-    <cfRule type="containsText" dxfId="32" priority="108" operator="containsText" text="Blocked">
+    <cfRule type="containsText" dxfId="92" priority="168" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",J31)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J31">
-    <cfRule type="containsText" dxfId="31" priority="106" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="91" priority="166" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",J31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="107" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="90" priority="167" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",J31)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J21">
-    <cfRule type="containsText" dxfId="29" priority="120" operator="containsText" text="Blocked">
+    <cfRule type="containsText" dxfId="89" priority="180" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",J21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J21">
-    <cfRule type="containsText" dxfId="28" priority="118" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="88" priority="178" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",J21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="119" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="87" priority="179" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",J21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J23 J25 J27">
-    <cfRule type="containsText" dxfId="26" priority="117" operator="containsText" text="Blocked">
+    <cfRule type="containsText" dxfId="86" priority="177" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",J23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J23 J25 J27">
-    <cfRule type="containsText" dxfId="25" priority="115" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="85" priority="175" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",J23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="116" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="84" priority="176" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",J23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J29">
-    <cfRule type="containsText" dxfId="23" priority="114" operator="containsText" text="Blocked">
+    <cfRule type="containsText" dxfId="83" priority="174" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",J29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J29">
-    <cfRule type="containsText" dxfId="22" priority="112" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="82" priority="172" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",J29)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="113" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="81" priority="173" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",J29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J88">
-    <cfRule type="containsText" dxfId="20" priority="63" operator="containsText" text="Blocked">
+    <cfRule type="containsText" dxfId="80" priority="123" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",J88)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J88">
-    <cfRule type="containsText" dxfId="19" priority="61" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="79" priority="121" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",J88)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="62" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="78" priority="122" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",J88)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4">
-    <cfRule type="containsText" dxfId="17" priority="60" operator="containsText" text="Blocked">
+    <cfRule type="containsText" dxfId="77" priority="57" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",J4)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="76" priority="58" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="75" priority="59" operator="equal">
+      <formula>"Passed"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="74" priority="60" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",J4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="73" priority="120" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",J4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4">
-    <cfRule type="containsText" dxfId="16" priority="58" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="72" priority="118" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",J4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="59" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="71" priority="119" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",J4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J6">
-    <cfRule type="containsText" dxfId="14" priority="15" operator="containsText" text="Blocked">
+    <cfRule type="containsText" dxfId="55" priority="50" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",J6)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="54" priority="51" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="53" priority="52" operator="equal">
+      <formula>"Passed"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="52" priority="53" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",J6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="51" priority="56" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",J6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J6">
-    <cfRule type="containsText" dxfId="13" priority="13" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="50" priority="54" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",J6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="14" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="49" priority="55" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",J6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8">
-    <cfRule type="containsText" dxfId="11" priority="12" operator="containsText" text="Blocked">
+    <cfRule type="containsText" dxfId="48" priority="43" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",J8)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="47" priority="44" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="46" priority="45" operator="equal">
+      <formula>"Passed"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="45" priority="46" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",J8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="44" priority="49" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",J8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8">
-    <cfRule type="containsText" dxfId="10" priority="10" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="43" priority="47" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",J8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="11" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="42" priority="48" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",J8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J10">
-    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="Blocked">
+    <cfRule type="containsText" dxfId="41" priority="36" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",J10)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="40" priority="37" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="39" priority="38" operator="equal">
+      <formula>"Passed"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="38" priority="39" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",J10)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="37" priority="42" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",J10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J10">
-    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="36" priority="40" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",J10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="35" priority="41" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",J10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12">
-    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="Blocked">
+    <cfRule type="containsText" dxfId="34" priority="29" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",J12)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="33" priority="30" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="32" priority="31" operator="equal">
+      <formula>"Passed"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="31" priority="32" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",J12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="30" priority="35" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",J12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12">
-    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="29" priority="33" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",J12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="5" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="28" priority="34" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",J12)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J14 J16 J18 J20 J22 J24 J26 J28 J30 J32">
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="Blocked">
+  <conditionalFormatting sqref="J14">
+    <cfRule type="containsText" dxfId="27" priority="22" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",J14)))</formula>
     </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="23" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="24" operator="equal">
+      <formula>"Passed"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="24" priority="25" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",J14)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="23" priority="28" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",J14)))</formula>
+    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J14 J16 J18 J20 J22 J24 J26 J28 J30 J32">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Failed">
+  <conditionalFormatting sqref="J14">
+    <cfRule type="containsText" dxfId="22" priority="26" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",J14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="21" priority="27" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",J14)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="15">
+  <conditionalFormatting sqref="J16">
+    <cfRule type="containsText" dxfId="20" priority="15" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",J16)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="16" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="17" operator="equal">
+      <formula>"Passed"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="17" priority="18" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",J16)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="16" priority="21" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",J16)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J16">
+    <cfRule type="containsText" dxfId="15" priority="19" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",J16)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="14" priority="20" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",J16)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J32">
+    <cfRule type="containsText" dxfId="13" priority="8" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",J32)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="9" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
+      <formula>"Passed"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",J32)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="14" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",J32)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J32">
+    <cfRule type="containsText" dxfId="8" priority="12" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",J32)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="13" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",J32)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J18 J20 J22 J24 J26 J28 J30">
+    <cfRule type="containsText" dxfId="6" priority="1" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",J18)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+      <formula>"Passed"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",J18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="7" operator="containsText" text="Blocked">
+      <formula>NOT(ISERROR(SEARCH("Blocked",J18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J18 J20 J22 J24 J26 J28 J30">
+    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",J18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="6" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",J18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="14">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Độ ưu tiên" prompt="Vui lòng lựa chọn độ ưu tiên cho test case này theo danh sách bên dưới:_x000a__x000a_Low: độ ưu tiên thấp._x000a_Medium: độ ưu tiên trung bình._x000a_High: độ ưu tiên cao._x000a_Critical: độ ưu tiên cực kỳ quan trọng, cần hoàn thành gấp." sqref="D4 D6 D32 D10 D12 D14 D16 D18 D20 D22 D24 D26 D28 D30" xr:uid="{0B3B9C58-D186-41EE-8D31-CF7DE61E8969}">
       <formula1>"Low, Medium, High, Critical"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Kết quả kiểm thử" prompt="Vui lòng lựa chọn kết quả kiểm thử cho test case này theo danh sách bên dưới:_x000a__x000a_Passed: kết quả thực thế khớp với kết quả mong đợi._x000a_Failed: kết quả thực thế không khớp với kết quả mong._x000a_Blocked: không thể so sánh do tính năng đã bị chặn." sqref="J4 J12 J6 J14 J10 J16 J18 J20 J22 J24 J26 J28 J30 J32" xr:uid="{C15833E6-0946-45BE-A470-BF64802D835B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Kết quả kiểm thử" prompt="Vui lòng lựa chọn kết quả kiểm thử cho test case này theo danh sách bên dưới:_x000a__x000a_Passed: kết quả thực thế khớp với kết quả mong đợi._x000a_Failed: kết quả thực thế không khớp với kết quả mong._x000a_Blocked: không thể so sánh do tính năng đã bị chặn." sqref="J4 J10 J16 J12 J8 J14 J20 J22 J24 J26 J28 J30 J32 J6 J18" xr:uid="{C15833E6-0946-45BE-A470-BF64802D835B}">
       <formula1>"Passed, Failed, Blocked"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Độ ưu tiên của test case." prompt="Quyết định thứ tự và độ quan trọng cần phải thực hiện của test case._x000a__x000a_Ví dụ: hệ thống bán hành thì những chức năng về bán hàng sẽ có độ ưu tiên cao." sqref="D2" xr:uid="{9B18BDDB-2737-4C5C-BCD8-633CA067FE2C}"/>
@@ -3245,9 +5525,6 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Chức năng chính của test case." prompt="Mỗi chức năng sẽ bao gồm nhiều test case khác nhau._x000a__x000a_Ví dụ: Chức năng [Đăng nhập]" sqref="B2" xr:uid="{8B593658-D535-4901-BEC5-08681B396715}"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Độ ưu tiên của test case." prompt="Vui lòng lựa chọn độ ưu tiên cho test case này theo danh sách bên dưới:_x000a__x000a_Low: độ ưu tiên thấp._x000a_Medium: độ ưu tiên trung bình._x000a_High: độ ưu tiên cao._x000a_Critical: độ ưu tiên cực kỳ quan trọng, cần hoàn thành gấp." sqref="D8" xr:uid="{6B36BC76-1AC3-41A5-8518-62E512D8A3D2}">
       <formula1>"Low, Medium, High, Critical"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Kết quả kiểm thử của test case." prompt="Vui lòng lựa chọn kết quả kiểm thử cho test case này theo danh sách bên dưới:_x000a__x000a_Passed: kết quả thực thế khớp với kết quả mong đợi._x000a_Failed: kết quả thực thế không khớp với kết quả mong._x000a_Blocked: không thể so sánh do tính năng đã bị chặn." sqref="J8" xr:uid="{398A31AA-65B9-4059-8C41-6A1325D503F0}">
-      <formula1>"Passed, Failed, Blocked"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Điều kiện tiên quyết." prompt="Trước khi thực hiện test case cần phải có những dữ liệu đầu vào là gì._x000a__x000a_Ví dụ: để có thể tiến hành đăng nhập thành công thì cần phải có tài khoản và mật khẩu hợp lệ." sqref="E2" xr:uid="{61B845AE-04F3-4D1A-B9BE-A3EAE2EDF92E}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Bước trước đó." prompt="Trước khi thực hiện test case cần phải có những bước nào._x000a__x000a_Ví dụ: để có thể chỉnh sửa thông tin cá nhân của tài khoản, cần phải đăng nhập thành công -&gt; chọn tính năng [Chỉnh sửa thông tin]." sqref="F2" xr:uid="{4F61F45A-19C3-4911-B60A-37C130716971}"/>

</xml_diff>